<commit_message>
added stuff and readme
</commit_message>
<xml_diff>
--- a/weight.xlsx
+++ b/weight.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkipust/My Drive/Homework/nlp/id_pos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D665E403-225B-FE42-986A-806CE86B0789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A262FC-12CC-C34C-9E0E-FAB086BE460C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="21340" windowHeight="18240" activeTab="3" xr2:uid="{5015098C-E6B9-A849-A57D-7436BC7D74E7}"/>
   </bookViews>
   <sheets>
     <sheet name="unaug" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Aug" sheetId="2" r:id="rId2"/>
     <sheet name="post_processing" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>global_emission_weight</t>
   </si>
@@ -110,12 +110,21 @@
   <si>
     <t>V</t>
   </si>
+  <si>
+    <t>g_transition</t>
+  </si>
+  <si>
+    <t>g_emission</t>
+  </si>
+  <si>
+    <t>weights</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,13 +132,182 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF77C47D"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81C77D"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6DC17C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF63BE7B"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5DB81"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBBD881"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB1D580"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA8D27F"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF94CD7E"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2E383"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8E082"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFDD82"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFECE683"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB84"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEDA80"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6E984"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDCA7D"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEE282"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDD27F"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCC27C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBB279"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBAA77"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBA175"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA9974"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9816F"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8796E"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8696B"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -144,8 +322,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1614,7 +1819,7 @@
           <c:invertIfNegative val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$101</c:f>
+              <c:f>Aug!$A$2:$A$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1923,7 +2128,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$101</c:f>
+              <c:f>Aug!$B$2:$B$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -2232,7 +2437,7 @@
           </c:yVal>
           <c:bubbleSize>
             <c:numRef>
-              <c:f>Sheet2!$F$2:$F$101</c:f>
+              <c:f>Aug!$F$2:$F$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -6201,10 +6406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57E80D6-DE01-7443-9D71-590606568141}">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:T101"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6912,7 +7117,7 @@
         <v>0.43749999999999217</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30</v>
       </c>
@@ -6933,7 +7138,7 @@
         <v>0.53125000000000477</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>30</v>
       </c>
@@ -6954,7 +7159,7 @@
         <v>0.53125000000000477</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>30</v>
       </c>
@@ -6975,7 +7180,7 @@
         <v>0.56250000000000788</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>30</v>
       </c>
@@ -6996,7 +7201,7 @@
         <v>0.59375000000001088</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>30</v>
       </c>
@@ -7017,7 +7222,7 @@
         <v>0.62500000000001399</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>30</v>
       </c>
@@ -7038,7 +7243,7 @@
         <v>0.62500000000001399</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>30</v>
       </c>
@@ -7059,7 +7264,7 @@
         <v>0.59375000000001088</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>30</v>
       </c>
@@ -7080,7 +7285,7 @@
         <v>0.53125000000000477</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>30</v>
       </c>
@@ -7101,7 +7306,7 @@
         <v>0.43749999999999217</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -7121,8 +7326,11 @@
         <f t="shared" si="0"/>
         <v>0.37500000000001654</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="P42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>40</v>
       </c>
@@ -7142,8 +7350,38 @@
         <f t="shared" si="0"/>
         <v>0.37500000000001654</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>10</v>
+      </c>
+      <c r="M43">
+        <v>20</v>
+      </c>
+      <c r="N43">
+        <v>30</v>
+      </c>
+      <c r="O43">
+        <v>40</v>
+      </c>
+      <c r="P43">
+        <v>50</v>
+      </c>
+      <c r="Q43">
+        <v>60</v>
+      </c>
+      <c r="R43">
+        <v>70</v>
+      </c>
+      <c r="S43">
+        <v>80</v>
+      </c>
+      <c r="T43">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>40</v>
       </c>
@@ -7163,8 +7401,41 @@
         <f t="shared" si="0"/>
         <v>0.46874999999999523</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0.94984647</v>
+      </c>
+      <c r="L44" s="5">
+        <v>0.94165814000000003</v>
+      </c>
+      <c r="M44" s="10">
+        <v>0.93858750999999996</v>
+      </c>
+      <c r="N44" s="15">
+        <v>0.93346980999999996</v>
+      </c>
+      <c r="O44" s="17">
+        <v>0.93142272000000004</v>
+      </c>
+      <c r="P44" s="20">
+        <v>0.93039917999999999</v>
+      </c>
+      <c r="Q44" s="17">
+        <v>0.93142272000000004</v>
+      </c>
+      <c r="R44" s="15">
+        <v>0.93346980999999996</v>
+      </c>
+      <c r="S44" s="17">
+        <v>0.93142272000000004</v>
+      </c>
+      <c r="T44" s="17">
+        <v>0.93142272000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>40</v>
       </c>
@@ -7184,8 +7455,41 @@
         <f t="shared" si="0"/>
         <v>0.49999999999999828</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>10</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0.94984647</v>
+      </c>
+      <c r="L45" s="5">
+        <v>0.94165814000000003</v>
+      </c>
+      <c r="M45" s="10">
+        <v>0.93858750999999996</v>
+      </c>
+      <c r="N45" s="16">
+        <v>0.93654042999999998</v>
+      </c>
+      <c r="O45" s="17">
+        <v>0.93142272000000004</v>
+      </c>
+      <c r="P45" s="20">
+        <v>0.93039917999999999</v>
+      </c>
+      <c r="Q45" s="15">
+        <v>0.93346980999999996</v>
+      </c>
+      <c r="R45" s="15">
+        <v>0.93346980999999996</v>
+      </c>
+      <c r="S45" s="15">
+        <v>0.93346980999999996</v>
+      </c>
+      <c r="T45" s="20">
+        <v>0.93039917999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>40</v>
       </c>
@@ -7205,8 +7509,41 @@
         <f t="shared" si="0"/>
         <v>0.53125000000000477</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>20</v>
+      </c>
+      <c r="K46" s="2">
+        <v>0.94882292999999995</v>
+      </c>
+      <c r="L46" s="5">
+        <v>0.94165814000000003</v>
+      </c>
+      <c r="M46" s="10">
+        <v>0.93858750999999996</v>
+      </c>
+      <c r="N46" s="16">
+        <v>0.93654042999999998</v>
+      </c>
+      <c r="O46" s="18">
+        <v>0.93449335</v>
+      </c>
+      <c r="P46" s="20">
+        <v>0.93039917999999999</v>
+      </c>
+      <c r="Q46" s="15">
+        <v>0.93346980999999996</v>
+      </c>
+      <c r="R46" s="15">
+        <v>0.93346980999999996</v>
+      </c>
+      <c r="S46" s="19">
+        <v>0.93244625999999997</v>
+      </c>
+      <c r="T46" s="23">
+        <v>0.92630502000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>40</v>
       </c>
@@ -7226,8 +7563,41 @@
         <f t="shared" si="0"/>
         <v>0.59375000000001088</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>30</v>
+      </c>
+      <c r="K47" s="1">
+        <v>0.94984647</v>
+      </c>
+      <c r="L47" s="6">
+        <v>0.94268167999999997</v>
+      </c>
+      <c r="M47" s="11">
+        <v>0.93961105</v>
+      </c>
+      <c r="N47" s="13">
+        <v>0.93756397000000002</v>
+      </c>
+      <c r="O47" s="14">
+        <v>0.93551689000000005</v>
+      </c>
+      <c r="P47" s="13">
+        <v>0.93756397000000002</v>
+      </c>
+      <c r="Q47" s="18">
+        <v>0.93449335</v>
+      </c>
+      <c r="R47" s="15">
+        <v>0.93346980999999996</v>
+      </c>
+      <c r="S47" s="20">
+        <v>0.93039917999999999</v>
+      </c>
+      <c r="T47" s="23">
+        <v>0.92630502000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>40</v>
       </c>
@@ -7247,8 +7617,41 @@
         <f t="shared" si="0"/>
         <v>0.59375000000001088</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J48">
+        <v>40</v>
+      </c>
+      <c r="K48" s="3">
+        <v>0.95087001000000004</v>
+      </c>
+      <c r="L48" s="7">
+        <v>0.94370522000000001</v>
+      </c>
+      <c r="M48" s="12">
+        <v>0.94063459999999999</v>
+      </c>
+      <c r="N48" s="10">
+        <v>0.93858750999999996</v>
+      </c>
+      <c r="O48" s="16">
+        <v>0.93654042999999998</v>
+      </c>
+      <c r="P48" s="10">
+        <v>0.93858750999999996</v>
+      </c>
+      <c r="Q48" s="13">
+        <v>0.93756397000000002</v>
+      </c>
+      <c r="R48" s="17">
+        <v>0.93142272000000004</v>
+      </c>
+      <c r="S48" s="17">
+        <v>0.93142272000000004</v>
+      </c>
+      <c r="T48" s="22">
+        <v>0.92732855999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>40</v>
       </c>
@@ -7268,8 +7671,44 @@
         <f t="shared" si="0"/>
         <v>0.46874999999999523</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I49" t="s">
+        <v>24</v>
+      </c>
+      <c r="J49">
+        <v>50</v>
+      </c>
+      <c r="K49" s="4">
+        <v>0.95189354999999998</v>
+      </c>
+      <c r="L49" s="8">
+        <v>0.94472875999999995</v>
+      </c>
+      <c r="M49" s="12">
+        <v>0.94063459999999999</v>
+      </c>
+      <c r="N49" s="11">
+        <v>0.93961105</v>
+      </c>
+      <c r="O49" s="10">
+        <v>0.93858750999999996</v>
+      </c>
+      <c r="P49" s="11">
+        <v>0.93961105</v>
+      </c>
+      <c r="Q49" s="14">
+        <v>0.93551689000000005</v>
+      </c>
+      <c r="R49" s="14">
+        <v>0.93551689000000005</v>
+      </c>
+      <c r="S49" s="15">
+        <v>0.93346980999999996</v>
+      </c>
+      <c r="T49" s="23">
+        <v>0.92630502000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>40</v>
       </c>
@@ -7289,8 +7728,41 @@
         <f t="shared" si="0"/>
         <v>0.4062500000000196</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J50">
+        <v>60</v>
+      </c>
+      <c r="K50" s="4">
+        <v>0.95189354999999998</v>
+      </c>
+      <c r="L50" s="9">
+        <v>0.94677584000000004</v>
+      </c>
+      <c r="M50" s="11">
+        <v>0.93961105</v>
+      </c>
+      <c r="N50" s="11">
+        <v>0.93961105</v>
+      </c>
+      <c r="O50" s="10">
+        <v>0.93858750999999996</v>
+      </c>
+      <c r="P50" s="14">
+        <v>0.93551689000000005</v>
+      </c>
+      <c r="Q50" s="14">
+        <v>0.93551689000000005</v>
+      </c>
+      <c r="R50" s="14">
+        <v>0.93551689000000005</v>
+      </c>
+      <c r="S50" s="15">
+        <v>0.93346980999999996</v>
+      </c>
+      <c r="T50" s="22">
+        <v>0.92732855999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>40</v>
       </c>
@@ -7310,8 +7782,41 @@
         <f t="shared" si="0"/>
         <v>0.4062500000000196</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J51">
+        <v>70</v>
+      </c>
+      <c r="K51" s="3">
+        <v>0.95087001000000004</v>
+      </c>
+      <c r="L51" s="9">
+        <v>0.94677584000000004</v>
+      </c>
+      <c r="M51" s="11">
+        <v>0.93961105</v>
+      </c>
+      <c r="N51" s="10">
+        <v>0.93858750999999996</v>
+      </c>
+      <c r="O51" s="18">
+        <v>0.93449335</v>
+      </c>
+      <c r="P51" s="18">
+        <v>0.93449335</v>
+      </c>
+      <c r="Q51" s="18">
+        <v>0.93449335</v>
+      </c>
+      <c r="R51" s="18">
+        <v>0.93449335</v>
+      </c>
+      <c r="S51" s="17">
+        <v>0.93142272000000004</v>
+      </c>
+      <c r="T51" s="25">
+        <v>0.92221085000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -7331,8 +7836,41 @@
         <f t="shared" si="0"/>
         <v>0.34375000000001005</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J52">
+        <v>80</v>
+      </c>
+      <c r="K52" s="2">
+        <v>0.94882292999999995</v>
+      </c>
+      <c r="L52" s="7">
+        <v>0.94370522000000001</v>
+      </c>
+      <c r="M52" s="13">
+        <v>0.93756397000000002</v>
+      </c>
+      <c r="N52" s="16">
+        <v>0.93654042999999998</v>
+      </c>
+      <c r="O52" s="19">
+        <v>0.93244625999999997</v>
+      </c>
+      <c r="P52" s="19">
+        <v>0.93244625999999997</v>
+      </c>
+      <c r="Q52" s="19">
+        <v>0.93244625999999997</v>
+      </c>
+      <c r="R52" s="22">
+        <v>0.92732855999999997</v>
+      </c>
+      <c r="S52" s="24">
+        <v>0.92528147000000005</v>
+      </c>
+      <c r="T52" s="26">
+        <v>0.92118730999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>50</v>
       </c>
@@ -7352,8 +7890,41 @@
         <f t="shared" si="0"/>
         <v>0.34375000000001005</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J53">
+        <v>90</v>
+      </c>
+      <c r="K53" s="2">
+        <v>0.94882292999999995</v>
+      </c>
+      <c r="L53" s="7">
+        <v>0.94370522000000001</v>
+      </c>
+      <c r="M53" s="14">
+        <v>0.93551689000000005</v>
+      </c>
+      <c r="N53" s="15">
+        <v>0.93346980999999996</v>
+      </c>
+      <c r="O53" s="19">
+        <v>0.93244625999999997</v>
+      </c>
+      <c r="P53" s="15">
+        <v>0.93346980999999996</v>
+      </c>
+      <c r="Q53" s="21">
+        <v>0.92835210000000001</v>
+      </c>
+      <c r="R53" s="23">
+        <v>0.92630502000000003</v>
+      </c>
+      <c r="S53" s="25">
+        <v>0.92221085000000003</v>
+      </c>
+      <c r="T53" s="27">
+        <v>0.91914023</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>50</v>
       </c>
@@ -7374,7 +7945,7 @@
         <v>0.34375000000001005</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>50</v>
       </c>
@@ -7395,7 +7966,7 @@
         <v>0.56250000000000788</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>50</v>
       </c>
@@ -7416,7 +7987,7 @@
         <v>0.59375000000001088</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>50</v>
       </c>
@@ -7437,7 +8008,7 @@
         <v>0.62500000000001399</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>50</v>
       </c>
@@ -7458,7 +8029,7 @@
         <v>0.49999999999999828</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>50</v>
       </c>
@@ -7479,7 +8050,7 @@
         <v>0.46874999999999523</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>50</v>
       </c>
@@ -7500,7 +8071,7 @@
         <v>0.4062500000000196</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>50</v>
       </c>
@@ -7521,7 +8092,7 @@
         <v>0.43749999999999217</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
@@ -7542,7 +8113,7 @@
         <v>0.37500000000001654</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>60</v>
       </c>
@@ -7563,7 +8134,7 @@
         <v>0.43749999999999217</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>60</v>
       </c>
@@ -8381,10 +8952,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A075EDBB-9625-3544-A0E2-D0D82A79D7B7}">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:U101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K2"/>
+    <sheetView topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31:U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8762,7 +9333,7 @@
         <v>0.60714285714285077</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>10</v>
       </c>
@@ -8783,7 +9354,7 @@
         <v>0.60714285714285077</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>10</v>
       </c>
@@ -8804,7 +9375,7 @@
         <v>0.60714285714285077</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>10</v>
       </c>
@@ -8825,7 +9396,7 @@
         <v>0.57142857142856207</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>10</v>
       </c>
@@ -8846,7 +9417,7 @@
         <v>0.53571428571427326</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10</v>
       </c>
@@ -8867,7 +9438,7 @@
         <v>0.53571428571427326</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -8888,7 +9459,7 @@
         <v>0.7857142857142636</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -8909,7 +9480,7 @@
         <v>0.64285714285713957</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>
@@ -8930,7 +9501,7 @@
         <v>0.60714285714285077</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20</v>
       </c>
@@ -8951,7 +9522,7 @@
         <v>0.50000000000001554</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
@@ -8972,7 +9543,7 @@
         <v>0.50000000000001554</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20</v>
       </c>
@@ -8993,7 +9564,7 @@
         <v>0.46428571428572674</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20</v>
       </c>
@@ -9014,7 +9585,7 @@
         <v>0.50000000000001554</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20</v>
       </c>
@@ -9035,7 +9606,7 @@
         <v>0.46428571428572674</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20</v>
       </c>
@@ -9056,7 +9627,7 @@
         <v>0.39285714285714923</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20</v>
       </c>
@@ -9076,8 +9647,14 @@
         <f t="shared" si="0"/>
         <v>0.39285714285714923</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J31" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -9097,8 +9674,38 @@
         <f t="shared" si="0"/>
         <v>0.67857142857142827</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>10</v>
+      </c>
+      <c r="N32">
+        <v>20</v>
+      </c>
+      <c r="O32">
+        <v>30</v>
+      </c>
+      <c r="P32">
+        <v>40</v>
+      </c>
+      <c r="Q32">
+        <v>50</v>
+      </c>
+      <c r="R32">
+        <v>60</v>
+      </c>
+      <c r="S32">
+        <v>70</v>
+      </c>
+      <c r="T32">
+        <v>80</v>
+      </c>
+      <c r="U32">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30</v>
       </c>
@@ -9118,8 +9725,41 @@
         <f t="shared" si="0"/>
         <v>0.53571428571427326</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0.93961105424769698</v>
+      </c>
+      <c r="M33">
+        <v>0.93244626407369502</v>
+      </c>
+      <c r="N33">
+        <v>0.933469805527123</v>
+      </c>
+      <c r="O33">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="P33">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="Q33">
+        <v>0.92732855680655002</v>
+      </c>
+      <c r="R33">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="S33">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="T33">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="U33">
+        <v>0.923234390992835</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>30</v>
       </c>
@@ -9139,8 +9779,41 @@
         <f t="shared" si="0"/>
         <v>0.53571428571427326</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <v>10</v>
+      </c>
+      <c r="L34">
+        <v>0.92118730808597704</v>
+      </c>
+      <c r="M34">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="N34">
+        <v>0.92937563971340797</v>
+      </c>
+      <c r="O34">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="P34">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="Q34">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="R34">
+        <v>0.923234390992835</v>
+      </c>
+      <c r="S34">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="T34">
+        <v>0.92118730808597704</v>
+      </c>
+      <c r="U34">
+        <v>0.92118730808597704</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>30</v>
       </c>
@@ -9160,8 +9833,41 @@
         <f t="shared" si="0"/>
         <v>0.53571428571427326</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <v>20</v>
+      </c>
+      <c r="L35">
+        <v>0.92221084953940602</v>
+      </c>
+      <c r="M35">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="N35">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="O35">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="P35">
+        <v>0.92732855680655002</v>
+      </c>
+      <c r="Q35">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="R35">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="S35">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="T35">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="U35">
+        <v>0.92016376663254795</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>30</v>
       </c>
@@ -9181,8 +9887,41 @@
         <f t="shared" si="0"/>
         <v>0.57142857142856207</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <v>30</v>
+      </c>
+      <c r="L36">
+        <v>0.92118730808597704</v>
+      </c>
+      <c r="M36">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="N36">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="O36">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="P36">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="Q36">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="R36">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="S36">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="T36">
+        <v>0.923234390992835</v>
+      </c>
+      <c r="U36">
+        <v>0.92221084953940602</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>30</v>
       </c>
@@ -9202,8 +9941,41 @@
         <f t="shared" si="0"/>
         <v>0.50000000000001554</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <v>40</v>
+      </c>
+      <c r="L37">
+        <v>0.92221084953940602</v>
+      </c>
+      <c r="M37">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="N37">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="O37">
+        <v>0.92732855680655002</v>
+      </c>
+      <c r="P37">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="Q37">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="R37">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="S37">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="T37">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="U37">
+        <v>0.92016376663254795</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>30</v>
       </c>
@@ -9223,8 +9995,44 @@
         <f t="shared" si="0"/>
         <v>0.50000000000001554</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J38" t="s">
+        <v>24</v>
+      </c>
+      <c r="K38">
+        <v>50</v>
+      </c>
+      <c r="L38">
+        <v>0.92016376663254795</v>
+      </c>
+      <c r="M38">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="N38">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="O38">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="P38">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="Q38">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="R38">
+        <v>0.923234390992835</v>
+      </c>
+      <c r="S38">
+        <v>0.923234390992835</v>
+      </c>
+      <c r="T38">
+        <v>0.923234390992835</v>
+      </c>
+      <c r="U38">
+        <v>0.92016376663254795</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>30</v>
       </c>
@@ -9244,8 +10052,41 @@
         <f t="shared" si="0"/>
         <v>0.46428571428572674</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <v>60</v>
+      </c>
+      <c r="L39">
+        <v>0.92118730808597704</v>
+      </c>
+      <c r="M39">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="N39">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="O39">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="P39">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="Q39">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="R39">
+        <v>0.923234390992835</v>
+      </c>
+      <c r="S39">
+        <v>0.92118730808597704</v>
+      </c>
+      <c r="T39">
+        <v>0.92221084953940602</v>
+      </c>
+      <c r="U39">
+        <v>0.91914022517911897</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>30</v>
       </c>
@@ -9265,8 +10106,41 @@
         <f t="shared" si="0"/>
         <v>0.39285714285714923</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K40">
+        <v>70</v>
+      </c>
+      <c r="L40">
+        <v>0.91914022517911897</v>
+      </c>
+      <c r="M40">
+        <v>0.92732855680655002</v>
+      </c>
+      <c r="N40">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="O40">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="P40">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="Q40">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="R40">
+        <v>0.92118730808597704</v>
+      </c>
+      <c r="S40">
+        <v>0.92016376663254795</v>
+      </c>
+      <c r="T40">
+        <v>0.92016376663254795</v>
+      </c>
+      <c r="U40">
+        <v>0.91709314227226202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>30</v>
       </c>
@@ -9286,8 +10160,41 @@
         <f t="shared" si="0"/>
         <v>0.39285714285714923</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K41">
+        <v>80</v>
+      </c>
+      <c r="L41">
+        <v>0.91504605936540395</v>
+      </c>
+      <c r="M41">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="N41">
+        <v>0.92221084953940602</v>
+      </c>
+      <c r="O41">
+        <v>0.92221084953940602</v>
+      </c>
+      <c r="P41">
+        <v>0.92118730808597704</v>
+      </c>
+      <c r="Q41">
+        <v>0.92118730808597704</v>
+      </c>
+      <c r="R41">
+        <v>0.91811668372569</v>
+      </c>
+      <c r="S41">
+        <v>0.91811668372569</v>
+      </c>
+      <c r="T41">
+        <v>0.91606960081883304</v>
+      </c>
+      <c r="U41">
+        <v>0.91095189355168804</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -9307,8 +10214,41 @@
         <f t="shared" si="0"/>
         <v>0.60714285714285077</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K42">
+        <v>90</v>
+      </c>
+      <c r="L42">
+        <v>0.91606960081883304</v>
+      </c>
+      <c r="M42">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="N42">
+        <v>0.92221084953940602</v>
+      </c>
+      <c r="O42">
+        <v>0.92221084953940602</v>
+      </c>
+      <c r="P42">
+        <v>0.92118730808597704</v>
+      </c>
+      <c r="Q42">
+        <v>0.91914022517911897</v>
+      </c>
+      <c r="R42">
+        <v>0.92016376663254795</v>
+      </c>
+      <c r="S42">
+        <v>0.91709314227226202</v>
+      </c>
+      <c r="T42">
+        <v>0.91095189355168804</v>
+      </c>
+      <c r="U42">
+        <v>0.91095189355168804</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>40</v>
       </c>
@@ -9329,7 +10269,7 @@
         <v>0.46428571428572674</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>40</v>
       </c>
@@ -9350,7 +10290,7 @@
         <v>0.57142857142856207</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>40</v>
       </c>
@@ -9371,7 +10311,7 @@
         <v>0.60714285714285077</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>40</v>
       </c>
@@ -9392,7 +10332,7 @@
         <v>0.60714285714285077</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>40</v>
       </c>
@@ -9413,7 +10353,7 @@
         <v>0.53571428571427326</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>40</v>
       </c>
@@ -10549,6 +11489,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E101">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L33:U42">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -10567,10 +11519,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F088CA15-3DA1-8944-AB44-A02D589D8858}">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:T101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="E14" workbookViewId="0">
+      <selection activeCell="R51" sqref="R51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11288,7 +12240,7 @@
         <v>0.47368421052631371</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30</v>
       </c>
@@ -11309,7 +12261,7 @@
         <v>0.57894736842105898</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>30</v>
       </c>
@@ -11330,7 +12282,7 @@
         <v>0.63157894736843156</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>30</v>
       </c>
@@ -11351,7 +12303,7 @@
         <v>0.7368421052631825</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>30</v>
       </c>
@@ -11371,8 +12323,14 @@
         <f t="shared" si="0"/>
         <v>0.7368421052631825</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I36" t="s">
+        <v>26</v>
+      </c>
+      <c r="P36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>30</v>
       </c>
@@ -11392,8 +12350,38 @@
         <f t="shared" si="0"/>
         <v>0.7368421052631825</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>10</v>
+      </c>
+      <c r="M37">
+        <v>20</v>
+      </c>
+      <c r="N37">
+        <v>30</v>
+      </c>
+      <c r="O37">
+        <v>40</v>
+      </c>
+      <c r="P37">
+        <v>50</v>
+      </c>
+      <c r="Q37">
+        <v>60</v>
+      </c>
+      <c r="R37">
+        <v>70</v>
+      </c>
+      <c r="S37">
+        <v>80</v>
+      </c>
+      <c r="T37">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>30</v>
       </c>
@@ -11413,8 +12401,41 @@
         <f t="shared" si="0"/>
         <v>0.78947368421050379</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0.92425793244626397</v>
+      </c>
+      <c r="L38">
+        <v>0.93142272262026604</v>
+      </c>
+      <c r="M38">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="N38">
+        <v>0.92732855680655002</v>
+      </c>
+      <c r="O38">
+        <v>0.92732855680655002</v>
+      </c>
+      <c r="P38">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="Q38">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="R38">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="S38">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="T38">
+        <v>0.92630501535312104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>30</v>
       </c>
@@ -11434,8 +12455,41 @@
         <f t="shared" si="0"/>
         <v>0.84210526315787637</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J39">
+        <v>10</v>
+      </c>
+      <c r="K39">
+        <v>0.923234390992835</v>
+      </c>
+      <c r="L39">
+        <v>0.93142272262026604</v>
+      </c>
+      <c r="M39">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="N39">
+        <v>0.92937563971340797</v>
+      </c>
+      <c r="O39">
+        <v>0.92732855680655002</v>
+      </c>
+      <c r="P39">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="Q39">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="R39">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="S39">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="T39">
+        <v>0.92425793244626397</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>30</v>
       </c>
@@ -11455,8 +12509,41 @@
         <f t="shared" si="0"/>
         <v>0.63157894736843156</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J40">
+        <v>20</v>
+      </c>
+      <c r="K40">
+        <v>0.923234390992835</v>
+      </c>
+      <c r="L40">
+        <v>0.93244626407369502</v>
+      </c>
+      <c r="M40">
+        <v>0.93142272262026604</v>
+      </c>
+      <c r="N40">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="O40">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="P40">
+        <v>0.92937563971340797</v>
+      </c>
+      <c r="Q40">
+        <v>0.92732855680655002</v>
+      </c>
+      <c r="R40">
+        <v>0.92732855680655002</v>
+      </c>
+      <c r="S40">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="T40">
+        <v>0.923234390992835</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>30</v>
       </c>
@@ -11476,8 +12563,41 @@
         <f t="shared" si="0"/>
         <v>0.57894736842105898</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J41">
+        <v>30</v>
+      </c>
+      <c r="K41">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="L41">
+        <v>0.93449334698055198</v>
+      </c>
+      <c r="M41">
+        <v>0.93244626407369502</v>
+      </c>
+      <c r="N41">
+        <v>0.93244626407369502</v>
+      </c>
+      <c r="O41">
+        <v>0.93244626407369502</v>
+      </c>
+      <c r="P41">
+        <v>0.933469805527123</v>
+      </c>
+      <c r="Q41">
+        <v>0.93142272262026604</v>
+      </c>
+      <c r="R41">
+        <v>0.92732855680655002</v>
+      </c>
+      <c r="S41">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="T41">
+        <v>0.92425793244626397</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -11497,8 +12617,41 @@
         <f t="shared" si="0"/>
         <v>0.47368421052631371</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>40</v>
+      </c>
+      <c r="K42">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="L42">
+        <v>0.93551688843398095</v>
+      </c>
+      <c r="M42">
+        <v>0.93449334698055198</v>
+      </c>
+      <c r="N42">
+        <v>0.93244626407369502</v>
+      </c>
+      <c r="O42">
+        <v>0.93244626407369502</v>
+      </c>
+      <c r="P42">
+        <v>0.933469805527123</v>
+      </c>
+      <c r="Q42">
+        <v>0.93142272262026604</v>
+      </c>
+      <c r="R42">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="S42">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="T42">
+        <v>0.923234390992835</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>40</v>
       </c>
@@ -11518,8 +12671,44 @@
         <f t="shared" si="0"/>
         <v>0.47368421052631371</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I43" t="s">
+        <v>24</v>
+      </c>
+      <c r="J43">
+        <v>50</v>
+      </c>
+      <c r="K43">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="L43">
+        <v>0.93551688843398095</v>
+      </c>
+      <c r="M43">
+        <v>0.93551688843398095</v>
+      </c>
+      <c r="N43">
+        <v>0.93244626407369502</v>
+      </c>
+      <c r="O43">
+        <v>0.93244626407369502</v>
+      </c>
+      <c r="P43">
+        <v>0.93142272262026604</v>
+      </c>
+      <c r="Q43">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="R43">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="S43">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="T43">
+        <v>0.92118730808597704</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>40</v>
       </c>
@@ -11539,8 +12728,41 @@
         <f t="shared" si="0"/>
         <v>0.63157894736843156</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>60</v>
+      </c>
+      <c r="K44">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="L44">
+        <v>0.93551688843398095</v>
+      </c>
+      <c r="M44">
+        <v>0.93551688843398095</v>
+      </c>
+      <c r="N44">
+        <v>0.933469805527123</v>
+      </c>
+      <c r="O44">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="P44">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="Q44">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="R44">
+        <v>0.928352098259979</v>
+      </c>
+      <c r="S44">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="T44">
+        <v>0.92118730808597704</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>40</v>
       </c>
@@ -11560,8 +12782,41 @@
         <f t="shared" si="0"/>
         <v>0.7368421052631825</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>70</v>
+      </c>
+      <c r="K45">
+        <v>0.92732855680655002</v>
+      </c>
+      <c r="L45">
+        <v>0.93654042988741004</v>
+      </c>
+      <c r="M45">
+        <v>0.93654042988741004</v>
+      </c>
+      <c r="N45">
+        <v>0.93449334698055198</v>
+      </c>
+      <c r="O45">
+        <v>0.93244626407369502</v>
+      </c>
+      <c r="P45">
+        <v>0.93142272262026604</v>
+      </c>
+      <c r="Q45">
+        <v>0.93142272262026604</v>
+      </c>
+      <c r="R45">
+        <v>0.92937563971340797</v>
+      </c>
+      <c r="S45">
+        <v>0.92630501535312104</v>
+      </c>
+      <c r="T45">
+        <v>0.92118730808597704</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>40</v>
       </c>
@@ -11581,8 +12836,41 @@
         <f t="shared" si="0"/>
         <v>0.7368421052631825</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>80</v>
+      </c>
+      <c r="K46">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="L46">
+        <v>0.93449334698055198</v>
+      </c>
+      <c r="M46">
+        <v>0.93449334698055198</v>
+      </c>
+      <c r="N46">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="O46">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="P46">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="Q46">
+        <v>0.92937563971340797</v>
+      </c>
+      <c r="R46">
+        <v>0.92221084953940602</v>
+      </c>
+      <c r="S46">
+        <v>0.91914022517911897</v>
+      </c>
+      <c r="T46">
+        <v>0.91811668372569</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>40</v>
       </c>
@@ -11602,8 +12890,41 @@
         <f t="shared" si="0"/>
         <v>0.7368421052631825</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>90</v>
+      </c>
+      <c r="K47">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="L47">
+        <v>0.93756397134083902</v>
+      </c>
+      <c r="M47">
+        <v>0.93244626407369502</v>
+      </c>
+      <c r="N47">
+        <v>0.92937563971340797</v>
+      </c>
+      <c r="O47">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="P47">
+        <v>0.93039918116683695</v>
+      </c>
+      <c r="Q47">
+        <v>0.92528147389969295</v>
+      </c>
+      <c r="R47">
+        <v>0.92221084953940602</v>
+      </c>
+      <c r="S47">
+        <v>0.91811668372569</v>
+      </c>
+      <c r="T47">
+        <v>0.91811668372569</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>40</v>
       </c>
@@ -12739,6 +14060,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E101">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K38:T47">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -12760,7 +14093,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12960,7 +14293,7 @@
         <v>0.5</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -12980,7 +14313,7 @@
         <v>0.5</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C11">
         <v>0</v>

</xml_diff>